<commit_message>
Silkscreen fixes & PCBWay assembly files
</commit_message>
<xml_diff>
--- a/Boards/Single_board/CPL/JLC_Top.xlsx
+++ b/Boards/Single_board/CPL/JLC_Top.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12360"/>
+    <workbookView windowWidth="30720" windowHeight="13440"/>
   </bookViews>
   <sheets>
     <sheet name="Main_board-bottom-pos" sheetId="1" r:id="rId1"/>
@@ -1641,8 +1641,8 @@
   <sheetPr/>
   <dimension ref="A1:H130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -1698,10 +1698,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="5">
-        <v>173.47</v>
+        <v>165.1</v>
       </c>
       <c r="C3" s="5">
-        <v>-68.83</v>
+        <v>-61.976</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -1718,10 +1718,10 @@
         <v>8</v>
       </c>
       <c r="B4" s="5">
-        <v>141.6</v>
+        <v>142.748</v>
       </c>
       <c r="C4" s="5">
-        <v>-146.4</v>
+        <v>-149.606</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -1738,10 +1738,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="5">
-        <v>141.6</v>
+        <v>143.002</v>
       </c>
       <c r="C5" s="5">
-        <v>-152.2</v>
+        <v>-155.194</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>

</xml_diff>